<commit_message>
Solve bug in transport and make tests work only for world
</commit_message>
<xml_diff>
--- a/models/transport.xlsx
+++ b/models/transport.xlsx
@@ -19,6 +19,16 @@
     <definedName function="false" hidden="false" localSheetId="0" name="bateries_ratio_hib_lv" vbProcedure="false">Global!$B$26</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="saving_ratios_vehicles" vbProcedure="false">Global!$B$10:$B$22</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="saving_ratio_2wE" vbProcedure="false">Global!$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="elec_2w" vbProcedure="false">World!$B$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="energy_initial_inland_transport" vbProcedure="false">World!$B$58:$B$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="initial_energy_intensity_households_transport" vbProcedure="false">World!$B$81:$B$85</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="initial_households_demand" vbProcedure="false">World!$B$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="initial_household_vehicles" vbProcedure="false">World!$B$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="initial_percent_T_vehicles" vbProcedure="false">World!$B$35:$B$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="initial_vehicles_inland" vbProcedure="false">World!$B$12:$B$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="initial_Xt_inland" vbProcedure="false">World!$B$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="liq_4w" vbProcedure="false">World!$B$51</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="percent_H_vehicles_initial" vbProcedure="false">World!$B$26:$B$31</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -360,52 +370,412 @@
   </authors>
   <commentList>
     <comment ref="A3" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Data of number of vehicle from 'International Energy Agency (2016), Energy Technology Perspectives 2016, OECD/IEA, Paris, except the number of buses taken from Global Transportation Roadmap  
+https://onedrive.live.com/?authkey=%21AOvHG9y4Oi%5F0Cts&amp;id=5F88C4E00B2E665B%21409962&amp;cid=5F88C4E00B2E665B
+ </t>
+        </r>
+      </text>
     </comment>
     <comment ref="A5" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Profesor:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">elec= batery electric vehicle+plug in hybrid</t>
+        </r>
+      </text>
     </comment>
     <comment ref="A8" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Two and three  wheelers gasoline</t>
+        </r>
+      </text>
     </comment>
     <comment ref="A9" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">electric two ant three
+ wheelers
+</t>
+        </r>
+      </text>
     </comment>
     <comment ref="A12" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">heavy vehicles</t>
+        </r>
+      </text>
     </comment>
     <comment ref="A15" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">light cargo vehicles</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B19" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Profesor:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Data from: Global Transportation
+Energy and Climate
+Roadmap,International Council on Clean Transportation 2012.
+</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B22" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">no data for number of trains found</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B46" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">No data available for number to trains</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B47" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">dato a boleo no tengo datos de los tresnes, no se como desegregarlos</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B51" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Data from 'International Energy Agency (2016), Energy Technology Perspectives 2016, OECD/IEA, Paris,</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B55" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">datos elaborados, tomado los de la IEA pero prorrateando el consumo entre liquidos y electricidad según el numero de 2wheelers de cada tipo y el ahorro medio de los electricos
+Data from 'International Energy Agency (2016), Energy Technology Perspectives 2016, OECD/IEA, Paris,</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B69" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">estimation, no world data found</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B70" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">estimation, no world data found</t>
+        </r>
+      </text>
     </comment>
     <comment ref="B71" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">both types of energy liquids+electricity mixed</t>
+        </r>
+      </text>
     </comment>
     <comment ref="C70" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">marga:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">estimation, no world data found</t>
+        </r>
+      </text>
     </comment>
   </commentList>
 </comments>
@@ -1515,8 +1885,8 @@
   </sheetPr>
   <dimension ref="A1:DE107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10369,11 +10739,12 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>